<commit_message>
improvement kalkulasi hasil pja
</commit_message>
<xml_diff>
--- a/excels/Form 2 - Checklist Pre Job Activty.xlsx
+++ b/excels/Form 2 - Checklist Pre Job Activty.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11108"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/ecsms/excels/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{812CBE3D-8418-A845-B120-D20DB32EF80E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{691D3081-F686-8142-B3C3-CCDCC9532DC1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -628,7 +628,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -666,94 +666,97 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="justify" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1378,8 +1381,8 @@
   </sheetPr>
   <dimension ref="A1:I113"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:I4"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="G87" activeCellId="1" sqref="F87 G87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -1452,12 +1455,12 @@
       <c r="A12" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="22" t="s">
+      <c r="B12" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="24"/>
+      <c r="C12" s="43"/>
+      <c r="D12" s="43"/>
+      <c r="E12" s="44"/>
       <c r="F12" s="5" t="s">
         <v>6</v>
       </c>
@@ -1472,593 +1475,593 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="39">
+      <c r="A13" s="28">
         <v>1</v>
       </c>
-      <c r="B13" s="30" t="s">
+      <c r="B13" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="30"/>
-      <c r="D13" s="30"/>
-      <c r="E13" s="30"/>
-      <c r="F13" s="30"/>
-      <c r="G13" s="30"/>
-      <c r="H13" s="30"/>
-      <c r="I13" s="30"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="20"/>
     </row>
     <row r="14" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="39"/>
+      <c r="A14" s="28"/>
       <c r="B14" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="43" t="s">
+      <c r="C14" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="D14" s="44"/>
-      <c r="E14" s="45"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="24"/>
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
       <c r="I14" s="9"/>
     </row>
     <row r="15" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="39"/>
+      <c r="A15" s="28"/>
       <c r="B15" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="D15" s="19"/>
-      <c r="E15" s="20"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="27"/>
       <c r="F15" s="9"/>
       <c r="G15" s="9"/>
       <c r="H15" s="9"/>
       <c r="I15" s="9"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="39">
+      <c r="A16" s="28">
         <v>2</v>
       </c>
-      <c r="B16" s="34" t="s">
+      <c r="B16" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="35"/>
-      <c r="D16" s="35"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="36"/>
-      <c r="I16" s="37"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="37"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="37"/>
+      <c r="I16" s="38"/>
     </row>
     <row r="17" spans="1:9" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="39"/>
+      <c r="A17" s="28"/>
       <c r="B17" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="C17" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="D17" s="19"/>
-      <c r="E17" s="20"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="27"/>
       <c r="F17" s="9"/>
       <c r="G17" s="9"/>
       <c r="H17" s="9"/>
       <c r="I17" s="9"/>
     </row>
     <row r="18" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="39"/>
+      <c r="A18" s="28"/>
       <c r="B18" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="C18" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="D18" s="19"/>
-      <c r="E18" s="20"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="27"/>
       <c r="F18" s="9"/>
       <c r="G18" s="9"/>
       <c r="H18" s="9"/>
       <c r="I18" s="9"/>
     </row>
     <row r="19" spans="1:9" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="39"/>
+      <c r="A19" s="28"/>
       <c r="B19" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="18" t="s">
+      <c r="C19" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="D19" s="19"/>
-      <c r="E19" s="20"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="27"/>
       <c r="F19" s="9"/>
       <c r="G19" s="9"/>
       <c r="H19" s="9"/>
       <c r="I19" s="9"/>
     </row>
     <row r="20" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="39"/>
+      <c r="A20" s="28"/>
       <c r="B20" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="18" t="s">
+      <c r="C20" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="D20" s="19"/>
-      <c r="E20" s="20"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="27"/>
       <c r="F20" s="9"/>
       <c r="G20" s="9"/>
       <c r="H20" s="9"/>
       <c r="I20" s="9"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="39">
+      <c r="A21" s="28">
         <v>3</v>
       </c>
-      <c r="B21" s="30" t="s">
+      <c r="B21" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="30"/>
-      <c r="D21" s="30"/>
-      <c r="E21" s="30"/>
-      <c r="F21" s="31"/>
-      <c r="G21" s="31"/>
-      <c r="H21" s="31"/>
-      <c r="I21" s="31"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="21"/>
+      <c r="I21" s="21"/>
     </row>
     <row r="22" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="39"/>
+      <c r="A22" s="28"/>
       <c r="B22" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C22" s="25" t="s">
+      <c r="C22" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="D22" s="26"/>
-      <c r="E22" s="27"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="19"/>
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
       <c r="H22" s="9"/>
       <c r="I22" s="9"/>
     </row>
     <row r="23" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="39"/>
+      <c r="A23" s="28"/>
       <c r="B23" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="25" t="s">
+      <c r="C23" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="D23" s="26"/>
-      <c r="E23" s="27"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="19"/>
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
       <c r="H23" s="9"/>
       <c r="I23" s="9"/>
     </row>
     <row r="24" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="39"/>
+      <c r="A24" s="28"/>
       <c r="B24" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C24" s="25" t="s">
+      <c r="C24" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="D24" s="26"/>
-      <c r="E24" s="27"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="19"/>
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
       <c r="H24" s="9"/>
       <c r="I24" s="9"/>
     </row>
     <row r="25" spans="1:9" s="3" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="39"/>
+      <c r="A25" s="28"/>
       <c r="B25" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="25" t="s">
+      <c r="C25" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="D25" s="26"/>
-      <c r="E25" s="27"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="19"/>
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
       <c r="H25" s="9"/>
       <c r="I25" s="9"/>
     </row>
     <row r="26" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="39"/>
+      <c r="A26" s="28"/>
       <c r="B26" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C26" s="25" t="s">
+      <c r="C26" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="D26" s="26"/>
-      <c r="E26" s="27"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="19"/>
       <c r="F26" s="9"/>
       <c r="G26" s="9"/>
       <c r="H26" s="9"/>
       <c r="I26" s="9"/>
     </row>
     <row r="27" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="39"/>
+      <c r="A27" s="28"/>
       <c r="B27" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C27" s="25" t="s">
+      <c r="C27" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="D27" s="26"/>
-      <c r="E27" s="27"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="19"/>
       <c r="F27" s="9"/>
       <c r="G27" s="9"/>
       <c r="H27" s="9"/>
       <c r="I27" s="9"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="39">
+      <c r="A28" s="28">
         <v>4</v>
       </c>
-      <c r="B28" s="34" t="s">
+      <c r="B28" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="C28" s="35"/>
-      <c r="D28" s="35"/>
-      <c r="E28" s="35"/>
-      <c r="F28" s="36"/>
-      <c r="G28" s="36"/>
-      <c r="H28" s="36"/>
-      <c r="I28" s="37"/>
+      <c r="C28" s="36"/>
+      <c r="D28" s="36"/>
+      <c r="E28" s="36"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="38"/>
     </row>
     <row r="29" spans="1:9" s="3" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="39"/>
+      <c r="A29" s="28"/>
       <c r="B29" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C29" s="25" t="s">
+      <c r="C29" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="D29" s="26"/>
-      <c r="E29" s="27"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="19"/>
       <c r="F29" s="9"/>
       <c r="G29" s="9"/>
       <c r="H29" s="9"/>
       <c r="I29" s="9"/>
     </row>
     <row r="30" spans="1:9" s="3" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="39"/>
+      <c r="A30" s="28"/>
       <c r="B30" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C30" s="25" t="s">
+      <c r="C30" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="D30" s="26"/>
-      <c r="E30" s="27"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="19"/>
       <c r="F30" s="9"/>
       <c r="G30" s="9"/>
       <c r="H30" s="9"/>
       <c r="I30" s="9"/>
     </row>
     <row r="31" spans="1:9" s="3" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="39"/>
+      <c r="A31" s="28"/>
       <c r="B31" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C31" s="25" t="s">
+      <c r="C31" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="D31" s="26"/>
-      <c r="E31" s="27"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="19"/>
       <c r="F31" s="9"/>
       <c r="G31" s="9"/>
       <c r="H31" s="9"/>
       <c r="I31" s="9"/>
     </row>
     <row r="32" spans="1:9" s="3" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="39"/>
+      <c r="A32" s="28"/>
       <c r="B32" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C32" s="25" t="s">
+      <c r="C32" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="D32" s="26"/>
-      <c r="E32" s="27"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="19"/>
       <c r="F32" s="9"/>
       <c r="G32" s="9"/>
       <c r="H32" s="9"/>
       <c r="I32" s="9"/>
     </row>
     <row r="33" spans="1:9" s="3" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="39"/>
+      <c r="A33" s="28"/>
       <c r="B33" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C33" s="25" t="s">
+      <c r="C33" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="D33" s="26"/>
-      <c r="E33" s="27"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="19"/>
       <c r="F33" s="9"/>
       <c r="G33" s="9"/>
       <c r="H33" s="9"/>
       <c r="I33" s="9"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A34" s="39">
+      <c r="A34" s="28">
         <v>5</v>
       </c>
-      <c r="B34" s="30" t="s">
+      <c r="B34" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="C34" s="30"/>
-      <c r="D34" s="30"/>
-      <c r="E34" s="30"/>
-      <c r="F34" s="31"/>
-      <c r="G34" s="31"/>
-      <c r="H34" s="31"/>
-      <c r="I34" s="31"/>
+      <c r="C34" s="20"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="21"/>
+      <c r="H34" s="21"/>
+      <c r="I34" s="21"/>
     </row>
     <row r="35" spans="1:9" s="3" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="39"/>
+      <c r="A35" s="28"/>
       <c r="B35" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C35" s="25" t="s">
+      <c r="C35" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="D35" s="26"/>
-      <c r="E35" s="27"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="19"/>
       <c r="F35" s="9"/>
       <c r="G35" s="9"/>
       <c r="H35" s="9"/>
       <c r="I35" s="9"/>
     </row>
     <row r="36" spans="1:9" s="3" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="39"/>
+      <c r="A36" s="28"/>
       <c r="B36" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C36" s="25" t="s">
+      <c r="C36" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="D36" s="26"/>
-      <c r="E36" s="27"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="19"/>
       <c r="F36" s="9"/>
       <c r="G36" s="9"/>
       <c r="H36" s="9"/>
       <c r="I36" s="9"/>
     </row>
     <row r="37" spans="1:9" s="3" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="39"/>
+      <c r="A37" s="28"/>
       <c r="B37" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C37" s="25" t="s">
+      <c r="C37" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="D37" s="26"/>
-      <c r="E37" s="27"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="19"/>
       <c r="F37" s="9"/>
       <c r="G37" s="9"/>
       <c r="H37" s="9"/>
       <c r="I37" s="9"/>
     </row>
     <row r="38" spans="1:9" s="3" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="39"/>
+      <c r="A38" s="28"/>
       <c r="B38" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C38" s="25" t="s">
+      <c r="C38" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="D38" s="26"/>
-      <c r="E38" s="27"/>
+      <c r="D38" s="18"/>
+      <c r="E38" s="19"/>
       <c r="F38" s="9"/>
       <c r="G38" s="9"/>
       <c r="H38" s="9"/>
       <c r="I38" s="9"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A39" s="39">
+      <c r="A39" s="28">
         <v>6</v>
       </c>
-      <c r="B39" s="30" t="s">
+      <c r="B39" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="C39" s="30"/>
-      <c r="D39" s="30"/>
-      <c r="E39" s="30"/>
-      <c r="F39" s="31"/>
-      <c r="G39" s="31"/>
-      <c r="H39" s="31"/>
-      <c r="I39" s="31"/>
+      <c r="C39" s="20"/>
+      <c r="D39" s="20"/>
+      <c r="E39" s="20"/>
+      <c r="F39" s="21"/>
+      <c r="G39" s="21"/>
+      <c r="H39" s="21"/>
+      <c r="I39" s="21"/>
     </row>
     <row r="40" spans="1:9" s="3" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="39"/>
+      <c r="A40" s="28"/>
       <c r="B40" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C40" s="25" t="s">
+      <c r="C40" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="D40" s="26"/>
-      <c r="E40" s="27"/>
+      <c r="D40" s="18"/>
+      <c r="E40" s="19"/>
       <c r="F40" s="9"/>
       <c r="G40" s="9"/>
       <c r="H40" s="9"/>
       <c r="I40" s="9"/>
     </row>
     <row r="41" spans="1:9" s="3" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="39"/>
+      <c r="A41" s="28"/>
       <c r="B41" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C41" s="25" t="s">
+      <c r="C41" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="D41" s="26"/>
-      <c r="E41" s="27"/>
+      <c r="D41" s="18"/>
+      <c r="E41" s="19"/>
       <c r="F41" s="9"/>
       <c r="G41" s="9"/>
       <c r="H41" s="9"/>
       <c r="I41" s="9"/>
     </row>
     <row r="42" spans="1:9" s="3" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="39"/>
+      <c r="A42" s="28"/>
       <c r="B42" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C42" s="40" t="s">
+      <c r="C42" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="D42" s="41"/>
-      <c r="E42" s="42"/>
+      <c r="D42" s="30"/>
+      <c r="E42" s="31"/>
       <c r="F42" s="9"/>
       <c r="G42" s="9"/>
       <c r="H42" s="9"/>
       <c r="I42" s="9"/>
     </row>
     <row r="43" spans="1:9" s="3" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="39"/>
+      <c r="A43" s="28"/>
       <c r="B43" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C43" s="25" t="s">
+      <c r="C43" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="D43" s="26"/>
-      <c r="E43" s="27"/>
+      <c r="D43" s="18"/>
+      <c r="E43" s="19"/>
       <c r="F43" s="9"/>
       <c r="G43" s="9"/>
       <c r="H43" s="9"/>
       <c r="I43" s="9"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A44" s="39">
+      <c r="A44" s="28">
         <v>7</v>
       </c>
-      <c r="B44" s="30" t="s">
+      <c r="B44" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="C44" s="30"/>
-      <c r="D44" s="30"/>
-      <c r="E44" s="30"/>
-      <c r="F44" s="31"/>
-      <c r="G44" s="31"/>
-      <c r="H44" s="31"/>
-      <c r="I44" s="31"/>
+      <c r="C44" s="20"/>
+      <c r="D44" s="20"/>
+      <c r="E44" s="20"/>
+      <c r="F44" s="21"/>
+      <c r="G44" s="21"/>
+      <c r="H44" s="21"/>
+      <c r="I44" s="21"/>
     </row>
     <row r="45" spans="1:9" s="3" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="39"/>
+      <c r="A45" s="28"/>
       <c r="B45" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C45" s="25" t="s">
+      <c r="C45" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="D45" s="26"/>
-      <c r="E45" s="27"/>
+      <c r="D45" s="18"/>
+      <c r="E45" s="19"/>
       <c r="F45" s="9"/>
       <c r="G45" s="9"/>
       <c r="H45" s="9"/>
       <c r="I45" s="9"/>
     </row>
     <row r="46" spans="1:9" s="3" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="39"/>
+      <c r="A46" s="28"/>
       <c r="B46" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C46" s="25" t="s">
+      <c r="C46" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="D46" s="26"/>
-      <c r="E46" s="27"/>
+      <c r="D46" s="18"/>
+      <c r="E46" s="19"/>
       <c r="F46" s="9"/>
       <c r="G46" s="9"/>
       <c r="H46" s="9"/>
       <c r="I46" s="9"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A47" s="39">
+      <c r="A47" s="28">
         <v>8</v>
       </c>
-      <c r="B47" s="30" t="s">
+      <c r="B47" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C47" s="30"/>
-      <c r="D47" s="30"/>
-      <c r="E47" s="30"/>
-      <c r="F47" s="31"/>
-      <c r="G47" s="31"/>
-      <c r="H47" s="31"/>
-      <c r="I47" s="31"/>
+      <c r="C47" s="20"/>
+      <c r="D47" s="20"/>
+      <c r="E47" s="20"/>
+      <c r="F47" s="21"/>
+      <c r="G47" s="21"/>
+      <c r="H47" s="21"/>
+      <c r="I47" s="21"/>
     </row>
     <row r="48" spans="1:9" s="3" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="39"/>
+      <c r="A48" s="28"/>
       <c r="B48" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C48" s="25" t="s">
+      <c r="C48" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="D48" s="26"/>
-      <c r="E48" s="27"/>
+      <c r="D48" s="18"/>
+      <c r="E48" s="19"/>
       <c r="F48" s="9"/>
       <c r="G48" s="9"/>
       <c r="H48" s="9"/>
       <c r="I48" s="9"/>
     </row>
     <row r="49" spans="1:9" s="3" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="39"/>
+      <c r="A49" s="28"/>
       <c r="B49" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C49" s="25" t="s">
+      <c r="C49" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="D49" s="26"/>
-      <c r="E49" s="27"/>
+      <c r="D49" s="18"/>
+      <c r="E49" s="19"/>
       <c r="F49" s="9"/>
       <c r="G49" s="9"/>
       <c r="H49" s="9"/>
       <c r="I49" s="9"/>
     </row>
     <row r="50" spans="1:9" s="3" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="39"/>
+      <c r="A50" s="28"/>
       <c r="B50" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C50" s="25" t="s">
+      <c r="C50" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="D50" s="26"/>
-      <c r="E50" s="27"/>
+      <c r="D50" s="18"/>
+      <c r="E50" s="19"/>
       <c r="F50" s="9"/>
       <c r="G50" s="9"/>
       <c r="H50" s="9"/>
       <c r="I50" s="9"/>
     </row>
     <row r="51" spans="1:9" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="39"/>
+      <c r="A51" s="28"/>
       <c r="B51" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C51" s="25" t="s">
+      <c r="C51" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="D51" s="26"/>
-      <c r="E51" s="27"/>
+      <c r="D51" s="18"/>
+      <c r="E51" s="19"/>
       <c r="F51" s="9"/>
       <c r="G51" s="9"/>
       <c r="H51" s="9"/>
       <c r="I51" s="9"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A52" s="39"/>
-      <c r="B52" s="39" t="s">
+      <c r="A52" s="28"/>
+      <c r="B52" s="28" t="s">
         <v>19</v>
       </c>
       <c r="C52" s="8" t="s">
@@ -2072,510 +2075,510 @@
       <c r="I52" s="9"/>
     </row>
     <row r="53" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="39"/>
-      <c r="B53" s="39"/>
+      <c r="A53" s="28"/>
+      <c r="B53" s="28"/>
       <c r="C53" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D53" s="25" t="s">
+      <c r="D53" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="E53" s="27"/>
+      <c r="E53" s="19"/>
       <c r="F53" s="9"/>
       <c r="G53" s="9"/>
       <c r="H53" s="9"/>
       <c r="I53" s="9"/>
     </row>
     <row r="54" spans="1:9" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="39"/>
-      <c r="B54" s="39"/>
+      <c r="A54" s="28"/>
+      <c r="B54" s="28"/>
       <c r="C54" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D54" s="25" t="s">
+      <c r="D54" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="E54" s="27"/>
+      <c r="E54" s="19"/>
       <c r="F54" s="9"/>
       <c r="G54" s="9"/>
       <c r="H54" s="9"/>
       <c r="I54" s="9"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A55" s="39"/>
-      <c r="B55" s="39"/>
+      <c r="A55" s="28"/>
+      <c r="B55" s="28"/>
       <c r="C55" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D55" s="28" t="s">
+      <c r="D55" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="E55" s="29"/>
+      <c r="E55" s="41"/>
       <c r="F55" s="9"/>
       <c r="G55" s="9"/>
       <c r="H55" s="9"/>
       <c r="I55" s="9"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A56" s="39"/>
-      <c r="B56" s="39"/>
+      <c r="A56" s="28"/>
+      <c r="B56" s="28"/>
       <c r="C56" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D56" s="28" t="s">
+      <c r="D56" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="E56" s="29"/>
+      <c r="E56" s="41"/>
       <c r="F56" s="9"/>
       <c r="G56" s="9"/>
       <c r="H56" s="9"/>
       <c r="I56" s="9"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A57" s="39"/>
-      <c r="B57" s="39"/>
+      <c r="A57" s="28"/>
+      <c r="B57" s="28"/>
       <c r="C57" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D57" s="28" t="s">
+      <c r="D57" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="E57" s="29"/>
+      <c r="E57" s="41"/>
       <c r="F57" s="9"/>
       <c r="G57" s="9"/>
       <c r="H57" s="9"/>
       <c r="I57" s="9"/>
     </row>
     <row r="58" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="39"/>
-      <c r="B58" s="39"/>
+      <c r="A58" s="28"/>
+      <c r="B58" s="28"/>
       <c r="C58" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D58" s="25" t="s">
+      <c r="D58" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="E58" s="27"/>
+      <c r="E58" s="19"/>
       <c r="F58" s="9"/>
       <c r="G58" s="9"/>
       <c r="H58" s="9"/>
       <c r="I58" s="9"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A59" s="39"/>
-      <c r="B59" s="39"/>
+      <c r="A59" s="28"/>
+      <c r="B59" s="28"/>
       <c r="C59" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D59" s="28" t="s">
+      <c r="D59" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="E59" s="29"/>
+      <c r="E59" s="41"/>
       <c r="F59" s="9"/>
       <c r="G59" s="9"/>
       <c r="H59" s="9"/>
       <c r="I59" s="9"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A60" s="39"/>
-      <c r="B60" s="39"/>
+      <c r="A60" s="28"/>
+      <c r="B60" s="28"/>
       <c r="C60" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D60" s="28" t="s">
+      <c r="D60" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="E60" s="29"/>
+      <c r="E60" s="41"/>
       <c r="F60" s="9"/>
       <c r="G60" s="9"/>
       <c r="H60" s="9"/>
       <c r="I60" s="9"/>
     </row>
     <row r="61" spans="1:9" ht="69.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="39"/>
-      <c r="B61" s="39"/>
+      <c r="A61" s="28"/>
+      <c r="B61" s="28"/>
       <c r="C61" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D61" s="25" t="s">
+      <c r="D61" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="E61" s="27"/>
+      <c r="E61" s="19"/>
       <c r="F61" s="9"/>
       <c r="G61" s="9"/>
       <c r="H61" s="9"/>
       <c r="I61" s="9"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A62" s="39"/>
-      <c r="B62" s="39"/>
+      <c r="A62" s="28"/>
+      <c r="B62" s="28"/>
       <c r="C62" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D62" s="28" t="s">
+      <c r="D62" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="E62" s="29"/>
+      <c r="E62" s="41"/>
       <c r="F62" s="9"/>
       <c r="G62" s="9"/>
       <c r="H62" s="9"/>
       <c r="I62" s="9"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A63" s="39"/>
-      <c r="B63" s="39"/>
+      <c r="A63" s="28"/>
+      <c r="B63" s="28"/>
       <c r="C63" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D63" s="28" t="s">
+      <c r="D63" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="E63" s="29"/>
+      <c r="E63" s="41"/>
       <c r="F63" s="9"/>
       <c r="G63" s="9"/>
       <c r="H63" s="9"/>
       <c r="I63" s="9"/>
     </row>
     <row r="64" spans="1:9" s="3" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="39"/>
+      <c r="A64" s="28"/>
       <c r="B64" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C64" s="25" t="s">
+      <c r="C64" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="D64" s="26"/>
-      <c r="E64" s="27"/>
+      <c r="D64" s="18"/>
+      <c r="E64" s="19"/>
       <c r="F64" s="9"/>
       <c r="G64" s="9"/>
       <c r="H64" s="9"/>
       <c r="I64" s="9"/>
     </row>
     <row r="65" spans="1:9" s="3" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="39"/>
+      <c r="A65" s="28"/>
       <c r="B65" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="C65" s="25" t="s">
+      <c r="C65" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="D65" s="26"/>
-      <c r="E65" s="27"/>
+      <c r="D65" s="18"/>
+      <c r="E65" s="19"/>
       <c r="F65" s="9"/>
       <c r="G65" s="9"/>
       <c r="H65" s="9"/>
       <c r="I65" s="9"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A66" s="39">
+      <c r="A66" s="28">
         <v>9</v>
       </c>
-      <c r="B66" s="30" t="s">
+      <c r="B66" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="C66" s="30"/>
-      <c r="D66" s="30"/>
-      <c r="E66" s="30"/>
-      <c r="F66" s="31"/>
-      <c r="G66" s="31"/>
-      <c r="H66" s="31"/>
-      <c r="I66" s="31"/>
+      <c r="C66" s="20"/>
+      <c r="D66" s="20"/>
+      <c r="E66" s="20"/>
+      <c r="F66" s="21"/>
+      <c r="G66" s="21"/>
+      <c r="H66" s="21"/>
+      <c r="I66" s="21"/>
     </row>
     <row r="67" spans="1:9" s="3" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="39"/>
+      <c r="A67" s="28"/>
       <c r="B67" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C67" s="25" t="s">
+      <c r="C67" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="D67" s="26"/>
-      <c r="E67" s="27"/>
+      <c r="D67" s="18"/>
+      <c r="E67" s="19"/>
       <c r="F67" s="9"/>
       <c r="G67" s="9"/>
       <c r="H67" s="9"/>
       <c r="I67" s="9"/>
     </row>
     <row r="68" spans="1:9" s="3" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="39"/>
+      <c r="A68" s="28"/>
       <c r="B68" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C68" s="25" t="s">
+      <c r="C68" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="D68" s="26"/>
-      <c r="E68" s="27"/>
+      <c r="D68" s="18"/>
+      <c r="E68" s="19"/>
       <c r="F68" s="9"/>
       <c r="G68" s="9"/>
       <c r="H68" s="9"/>
       <c r="I68" s="9"/>
     </row>
     <row r="69" spans="1:9" s="3" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="39"/>
+      <c r="A69" s="28"/>
       <c r="B69" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C69" s="25" t="s">
+      <c r="C69" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="D69" s="26"/>
-      <c r="E69" s="27"/>
+      <c r="D69" s="18"/>
+      <c r="E69" s="19"/>
       <c r="F69" s="9"/>
       <c r="G69" s="9"/>
       <c r="H69" s="9"/>
       <c r="I69" s="9"/>
     </row>
     <row r="70" spans="1:9" s="3" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="39"/>
+      <c r="A70" s="28"/>
       <c r="B70" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C70" s="25" t="s">
+      <c r="C70" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="D70" s="26"/>
-      <c r="E70" s="27"/>
+      <c r="D70" s="18"/>
+      <c r="E70" s="19"/>
       <c r="F70" s="9"/>
       <c r="G70" s="9"/>
       <c r="H70" s="9"/>
       <c r="I70" s="9"/>
     </row>
     <row r="71" spans="1:9" s="3" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="39"/>
+      <c r="A71" s="28"/>
       <c r="B71" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C71" s="25" t="s">
+      <c r="C71" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="D71" s="26"/>
-      <c r="E71" s="27"/>
+      <c r="D71" s="18"/>
+      <c r="E71" s="19"/>
       <c r="F71" s="9"/>
       <c r="G71" s="9"/>
       <c r="H71" s="9"/>
       <c r="I71" s="9"/>
     </row>
     <row r="72" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="39">
+      <c r="A72" s="28">
         <v>10</v>
       </c>
-      <c r="B72" s="38" t="s">
+      <c r="B72" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="C72" s="38"/>
-      <c r="D72" s="38"/>
-      <c r="E72" s="38"/>
-      <c r="F72" s="31"/>
-      <c r="G72" s="31"/>
-      <c r="H72" s="31"/>
-      <c r="I72" s="31"/>
+      <c r="C72" s="39"/>
+      <c r="D72" s="39"/>
+      <c r="E72" s="39"/>
+      <c r="F72" s="21"/>
+      <c r="G72" s="21"/>
+      <c r="H72" s="21"/>
+      <c r="I72" s="21"/>
     </row>
     <row r="73" spans="1:9" s="4" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="39"/>
+      <c r="A73" s="28"/>
       <c r="B73" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C73" s="18" t="s">
+      <c r="C73" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="D73" s="19"/>
-      <c r="E73" s="20"/>
+      <c r="D73" s="26"/>
+      <c r="E73" s="27"/>
       <c r="F73" s="9"/>
       <c r="G73" s="9"/>
       <c r="H73" s="9"/>
       <c r="I73" s="9"/>
     </row>
     <row r="74" spans="1:9" s="4" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="39"/>
+      <c r="A74" s="28"/>
       <c r="B74" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C74" s="18" t="s">
+      <c r="C74" s="25" t="s">
         <v>89</v>
       </c>
-      <c r="D74" s="19"/>
-      <c r="E74" s="20"/>
+      <c r="D74" s="26"/>
+      <c r="E74" s="27"/>
       <c r="F74" s="9"/>
       <c r="G74" s="9"/>
       <c r="H74" s="9"/>
       <c r="I74" s="9"/>
     </row>
     <row r="75" spans="1:9" s="4" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="39"/>
+      <c r="A75" s="28"/>
       <c r="B75" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C75" s="18" t="s">
+      <c r="C75" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="D75" s="19"/>
-      <c r="E75" s="20"/>
+      <c r="D75" s="26"/>
+      <c r="E75" s="27"/>
       <c r="F75" s="9"/>
       <c r="G75" s="9"/>
       <c r="H75" s="9"/>
       <c r="I75" s="9"/>
     </row>
     <row r="76" spans="1:9" s="4" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="39"/>
+      <c r="A76" s="28"/>
       <c r="B76" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C76" s="18" t="s">
+      <c r="C76" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="D76" s="19"/>
-      <c r="E76" s="20"/>
+      <c r="D76" s="26"/>
+      <c r="E76" s="27"/>
       <c r="F76" s="9"/>
       <c r="G76" s="9"/>
       <c r="H76" s="9"/>
       <c r="I76" s="9"/>
     </row>
     <row r="77" spans="1:9" s="4" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="39"/>
+      <c r="A77" s="28"/>
       <c r="B77" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C77" s="18" t="s">
+      <c r="C77" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="D77" s="19"/>
-      <c r="E77" s="20"/>
+      <c r="D77" s="26"/>
+      <c r="E77" s="27"/>
       <c r="F77" s="9"/>
       <c r="G77" s="9"/>
       <c r="H77" s="9"/>
       <c r="I77" s="9"/>
     </row>
     <row r="78" spans="1:9" s="4" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="39"/>
+      <c r="A78" s="28"/>
       <c r="B78" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C78" s="18" t="s">
+      <c r="C78" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="D78" s="19"/>
-      <c r="E78" s="20"/>
+      <c r="D78" s="26"/>
+      <c r="E78" s="27"/>
       <c r="F78" s="9"/>
       <c r="G78" s="9"/>
       <c r="H78" s="9"/>
       <c r="I78" s="9"/>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A79" s="39">
+      <c r="A79" s="28">
         <v>11</v>
       </c>
-      <c r="B79" s="30" t="s">
+      <c r="B79" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="C79" s="30"/>
-      <c r="D79" s="30"/>
-      <c r="E79" s="30"/>
-      <c r="F79" s="31"/>
-      <c r="G79" s="31"/>
-      <c r="H79" s="31"/>
-      <c r="I79" s="31"/>
+      <c r="C79" s="20"/>
+      <c r="D79" s="20"/>
+      <c r="E79" s="20"/>
+      <c r="F79" s="21"/>
+      <c r="G79" s="21"/>
+      <c r="H79" s="21"/>
+      <c r="I79" s="21"/>
     </row>
     <row r="80" spans="1:9" s="3" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="39"/>
+      <c r="A80" s="28"/>
       <c r="B80" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C80" s="25" t="s">
+      <c r="C80" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="D80" s="26"/>
-      <c r="E80" s="27"/>
+      <c r="D80" s="18"/>
+      <c r="E80" s="19"/>
       <c r="F80" s="9"/>
       <c r="G80" s="9"/>
       <c r="H80" s="9"/>
       <c r="I80" s="9"/>
     </row>
     <row r="81" spans="1:9" s="3" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="39"/>
+      <c r="A81" s="28"/>
       <c r="B81" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C81" s="25" t="s">
+      <c r="C81" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="D81" s="26"/>
-      <c r="E81" s="27"/>
+      <c r="D81" s="18"/>
+      <c r="E81" s="19"/>
       <c r="F81" s="9"/>
       <c r="G81" s="9"/>
       <c r="H81" s="9"/>
       <c r="I81" s="9"/>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A82" s="39">
+      <c r="A82" s="28">
         <v>12</v>
       </c>
-      <c r="B82" s="30" t="s">
+      <c r="B82" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="C82" s="30"/>
-      <c r="D82" s="30"/>
-      <c r="E82" s="30"/>
-      <c r="F82" s="31"/>
-      <c r="G82" s="31"/>
-      <c r="H82" s="31"/>
-      <c r="I82" s="31"/>
+      <c r="C82" s="20"/>
+      <c r="D82" s="20"/>
+      <c r="E82" s="20"/>
+      <c r="F82" s="21"/>
+      <c r="G82" s="21"/>
+      <c r="H82" s="21"/>
+      <c r="I82" s="21"/>
     </row>
     <row r="83" spans="1:9" s="4" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="39"/>
+      <c r="A83" s="28"/>
       <c r="B83" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C83" s="18" t="s">
+      <c r="C83" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="D83" s="19"/>
-      <c r="E83" s="20"/>
+      <c r="D83" s="26"/>
+      <c r="E83" s="27"/>
       <c r="F83" s="9"/>
       <c r="G83" s="9"/>
       <c r="H83" s="9"/>
       <c r="I83" s="9"/>
     </row>
     <row r="84" spans="1:9" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="39"/>
+      <c r="A84" s="28"/>
       <c r="B84" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C84" s="18" t="s">
+      <c r="C84" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="D84" s="19"/>
-      <c r="E84" s="20"/>
+      <c r="D84" s="26"/>
+      <c r="E84" s="27"/>
       <c r="F84" s="9"/>
       <c r="G84" s="9"/>
       <c r="H84" s="9"/>
       <c r="I84" s="9"/>
     </row>
     <row r="85" spans="1:9" s="4" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="39"/>
+      <c r="A85" s="28"/>
       <c r="B85" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C85" s="18" t="s">
+      <c r="C85" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="D85" s="19"/>
-      <c r="E85" s="20"/>
+      <c r="D85" s="26"/>
+      <c r="E85" s="27"/>
       <c r="F85" s="9"/>
       <c r="G85" s="9"/>
       <c r="H85" s="9"/>
       <c r="I85" s="9"/>
     </row>
     <row r="86" spans="1:9" s="4" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="39"/>
+      <c r="A86" s="28"/>
       <c r="B86" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C86" s="18" t="s">
+      <c r="C86" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="D86" s="19"/>
-      <c r="E86" s="20"/>
+      <c r="D86" s="26"/>
+      <c r="E86" s="27"/>
       <c r="F86" s="9"/>
       <c r="G86" s="9"/>
       <c r="H86" s="9"/>
@@ -2589,8 +2592,8 @@
       <c r="C87" s="33"/>
       <c r="D87" s="33"/>
       <c r="E87" s="12"/>
-      <c r="F87" s="8"/>
-      <c r="G87" s="8"/>
+      <c r="F87" s="16"/>
+      <c r="G87" s="16"/>
     </row>
     <row r="88" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="8"/>
@@ -2600,8 +2603,8 @@
       <c r="C88" s="33"/>
       <c r="D88" s="33"/>
       <c r="E88" s="12"/>
-      <c r="F88" s="17"/>
-      <c r="G88" s="17"/>
+      <c r="F88" s="34"/>
+      <c r="G88" s="34"/>
     </row>
     <row r="94" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="95" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2615,38 +2618,38 @@
     </row>
     <row r="97" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="98" spans="1:9" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B98" s="21" t="s">
+      <c r="B98" s="46" t="s">
         <v>97</v>
       </c>
-      <c r="C98" s="21"/>
-      <c r="D98" s="21"/>
-      <c r="E98" s="21"/>
-      <c r="F98" s="21"/>
-      <c r="G98" s="21"/>
-      <c r="H98" s="21"/>
-      <c r="I98" s="21"/>
+      <c r="C98" s="46"/>
+      <c r="D98" s="46"/>
+      <c r="E98" s="46"/>
+      <c r="F98" s="46"/>
+      <c r="G98" s="46"/>
+      <c r="H98" s="46"/>
+      <c r="I98" s="46"/>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B100" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="E100" s="16" t="s">
+      <c r="E100" s="45" t="s">
         <v>101</v>
       </c>
-      <c r="F100" s="17" t="s">
+      <c r="F100" s="34" t="s">
         <v>107</v>
       </c>
-      <c r="G100" s="17"/>
-      <c r="H100" s="17" t="s">
+      <c r="G100" s="34"/>
+      <c r="H100" s="34" t="s">
         <v>108</v>
       </c>
-      <c r="I100" s="17"/>
+      <c r="I100" s="34"/>
     </row>
     <row r="101" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B101" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="E101" s="16"/>
+      <c r="E101" s="45"/>
       <c r="F101" s="9" t="s">
         <v>102</v>
       </c>
@@ -2661,14 +2664,14 @@
       </c>
     </row>
     <row r="102" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E102" s="16"/>
+      <c r="E102" s="45"/>
       <c r="F102" s="13"/>
       <c r="G102" s="13"/>
       <c r="H102" s="8"/>
       <c r="I102" s="8"/>
     </row>
     <row r="103" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E103" s="16"/>
+      <c r="E103" s="45"/>
       <c r="F103" s="13"/>
       <c r="G103" s="13"/>
       <c r="H103" s="8"/>
@@ -2720,34 +2723,57 @@
     </row>
   </sheetData>
   <mergeCells count="95">
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="B21:I21"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="A28:A33"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="A16:A20"/>
-    <mergeCell ref="A21:A27"/>
-    <mergeCell ref="A34:A38"/>
-    <mergeCell ref="A39:A43"/>
-    <mergeCell ref="A44:A46"/>
-    <mergeCell ref="A47:A65"/>
-    <mergeCell ref="B52:B63"/>
-    <mergeCell ref="C42:E42"/>
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="C45:E45"/>
-    <mergeCell ref="C46:E46"/>
-    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="E100:E103"/>
+    <mergeCell ref="F100:G100"/>
+    <mergeCell ref="H100:I100"/>
+    <mergeCell ref="C83:E83"/>
+    <mergeCell ref="C84:E84"/>
+    <mergeCell ref="C85:E85"/>
+    <mergeCell ref="C86:E86"/>
+    <mergeCell ref="B98:I98"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="C76:E76"/>
+    <mergeCell ref="C77:E77"/>
+    <mergeCell ref="C78:E78"/>
+    <mergeCell ref="C80:E80"/>
+    <mergeCell ref="C64:E64"/>
+    <mergeCell ref="C65:E65"/>
+    <mergeCell ref="C67:E67"/>
+    <mergeCell ref="C68:E68"/>
+    <mergeCell ref="C69:E69"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="C81:E81"/>
+    <mergeCell ref="C70:E70"/>
+    <mergeCell ref="C71:E71"/>
+    <mergeCell ref="C73:E73"/>
+    <mergeCell ref="C74:E74"/>
+    <mergeCell ref="C75:E75"/>
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="B34:I34"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="C48:E48"/>
+    <mergeCell ref="C49:E49"/>
+    <mergeCell ref="C50:E50"/>
+    <mergeCell ref="C51:E51"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="B39:I39"/>
+    <mergeCell ref="B44:I44"/>
+    <mergeCell ref="C40:E40"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="C33:E33"/>
+    <mergeCell ref="C35:E35"/>
     <mergeCell ref="A4:I4"/>
     <mergeCell ref="B88:D88"/>
     <mergeCell ref="F88:G88"/>
@@ -2764,57 +2790,34 @@
     <mergeCell ref="A79:A81"/>
     <mergeCell ref="A82:A86"/>
     <mergeCell ref="B13:I13"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="C31:E31"/>
-    <mergeCell ref="C32:E32"/>
-    <mergeCell ref="C33:E33"/>
-    <mergeCell ref="C35:E35"/>
-    <mergeCell ref="C36:E36"/>
-    <mergeCell ref="B34:I34"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="D56:E56"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="C48:E48"/>
-    <mergeCell ref="C49:E49"/>
-    <mergeCell ref="C50:E50"/>
-    <mergeCell ref="C51:E51"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="B39:I39"/>
-    <mergeCell ref="B44:I44"/>
-    <mergeCell ref="C40:E40"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="C37:E37"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C81:E81"/>
-    <mergeCell ref="C70:E70"/>
-    <mergeCell ref="C71:E71"/>
-    <mergeCell ref="C73:E73"/>
-    <mergeCell ref="C74:E74"/>
-    <mergeCell ref="C75:E75"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="C76:E76"/>
-    <mergeCell ref="C77:E77"/>
-    <mergeCell ref="C78:E78"/>
-    <mergeCell ref="C80:E80"/>
-    <mergeCell ref="C64:E64"/>
-    <mergeCell ref="C65:E65"/>
-    <mergeCell ref="C67:E67"/>
-    <mergeCell ref="C68:E68"/>
-    <mergeCell ref="C69:E69"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="D63:E63"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="E100:E103"/>
-    <mergeCell ref="F100:G100"/>
-    <mergeCell ref="H100:I100"/>
-    <mergeCell ref="C83:E83"/>
-    <mergeCell ref="C84:E84"/>
-    <mergeCell ref="C85:E85"/>
-    <mergeCell ref="C86:E86"/>
-    <mergeCell ref="B98:I98"/>
+    <mergeCell ref="A39:A43"/>
+    <mergeCell ref="A44:A46"/>
+    <mergeCell ref="A47:A65"/>
+    <mergeCell ref="B52:B63"/>
+    <mergeCell ref="C42:E42"/>
+    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="C45:E45"/>
+    <mergeCell ref="C46:E46"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="A28:A33"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="A16:A20"/>
+    <mergeCell ref="A21:A27"/>
+    <mergeCell ref="A34:A38"/>
+    <mergeCell ref="B21:I21"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="C26:E26"/>
   </mergeCells>
   <pageMargins left="0.59055118110236227" right="0.19685039370078741" top="0.39370078740157483" bottom="0.19685039370078741" header="0" footer="0"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
@@ -2823,18 +2826,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocId xmlns="f8ce19fc-6d1c-4a32-9ccc-c9d52d339ce3">JDHWM6R55FRK-3-1091</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="f8ce19fc-6d1c-4a32-9ccc-c9d52d339ce3">
-      <Url>http://intra-ecorr.pertamina.com:1043/sites/DIR/_layouts/DocIdRedir.aspx?ID=JDHWM6R55FRK-3-1091</Url>
-      <Description>JDHWM6R55FRK-3-1091</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D3398B66F6FF2D41BB4BC1F9AFA58185" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3a6c582f2b0bd71f194a9173d25feba3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f8ce19fc-6d1c-4a32-9ccc-c9d52d339ce3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bbc7d0c2066ec31eb77a1a91b3421a26" ns2:_="">
     <xsd:import namespace="f8ce19fc-6d1c-4a32-9ccc-c9d52d339ce3"/>
@@ -2979,7 +2970,28 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="f8ce19fc-6d1c-4a32-9ccc-c9d52d339ce3">JDHWM6R55FRK-3-1091</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="f8ce19fc-6d1c-4a32-9ccc-c9d52d339ce3">
+      <Url>http://intra-ecorr.pertamina.com:1043/sites/DIR/_layouts/DocIdRedir.aspx?ID=JDHWM6R55FRK-3-1091</Url>
+      <Description>JDHWM6R55FRK-3-1091</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -3025,26 +3037,7 @@
 </spe:Receivers>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F0FE8FF-1470-4D65-B8CB-44279A87CD25}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="f8ce19fc-6d1c-4a32-9ccc-c9d52d339ce3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50EAB68D-D504-41D1-82F9-E4C3C5838B05}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3062,18 +3055,28 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F0FE8FF-1470-4D65-B8CB-44279A87CD25}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="f8ce19fc-6d1c-4a32-9ccc-c9d52d339ce3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{63767986-64D3-45A1-BF8E-61CD1787B5FF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{25744CA3-91BF-4923-A10C-D92CF0741E21}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{63767986-64D3-45A1-BF8E-61CD1787B5FF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
unmerge pja xls pdf
</commit_message>
<xml_diff>
--- a/excels/Form 2 - Checklist Pre Job Activty.xlsx
+++ b/excels/Form 2 - Checklist Pre Job Activty.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/ecsms/excels/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F606A04A-10D8-E648-A5AD-ABF135FC77A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CDF0250-D99F-F040-872D-254A652D8712}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="115">
   <si>
     <t>Lampiran 8 - Pedoman No. A-001/K00100/2015-S9 Rev.03</t>
   </si>
@@ -498,6 +498,9 @@
   </si>
   <si>
     <t>∑ Pokok Bahasan yang dicheck (YA + TIDAK)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -689,7 +692,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -727,127 +730,137 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1132,10 +1145,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I113"/>
+  <dimension ref="A1:I116"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A84" workbookViewId="0">
-      <selection activeCell="K105" sqref="K105"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A86" workbookViewId="0">
+      <selection activeCell="D101" sqref="D101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -1152,99 +1165,99 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
     </row>
     <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
+      <c r="B4" s="52"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="52"/>
+      <c r="H4" s="52"/>
+      <c r="I4" s="52"/>
     </row>
     <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="56" t="s">
+      <c r="B6" s="31"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="E6" s="56"/>
-      <c r="F6" s="56"/>
-      <c r="G6" s="56"/>
-      <c r="H6" s="56"/>
-      <c r="I6" s="56"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30"/>
     </row>
     <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28" t="s">
+      <c r="B7" s="31"/>
+      <c r="C7" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="D7" s="56" t="s">
+      <c r="D7" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="E7" s="56"/>
-      <c r="F7" s="56"/>
-      <c r="G7" s="56"/>
-      <c r="H7" s="56"/>
-      <c r="I7" s="56"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="30"/>
+      <c r="I7" s="30"/>
     </row>
     <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="28"/>
-      <c r="C8" s="28" t="s">
+      <c r="B8" s="31"/>
+      <c r="C8" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="D8" s="56" t="s">
+      <c r="D8" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="E8" s="56"/>
-      <c r="F8" s="56"/>
-      <c r="G8" s="56"/>
-      <c r="H8" s="56"/>
-      <c r="I8" s="56"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="30"/>
+      <c r="I8" s="30"/>
     </row>
     <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="28"/>
-      <c r="C9" s="28" t="s">
+      <c r="B9" s="31"/>
+      <c r="C9" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="D9" s="56" t="s">
+      <c r="D9" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="E9" s="56"/>
-      <c r="F9" s="56"/>
-      <c r="G9" s="56"/>
-      <c r="H9" s="56"/>
-      <c r="I9" s="56"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="30"/>
+      <c r="H9" s="30"/>
+      <c r="I9" s="30"/>
     </row>
     <row r="12" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
@@ -1270,22 +1283,22 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="37">
+      <c r="A13" s="18">
         <v>1</v>
       </c>
-      <c r="B13" s="32" t="s">
+      <c r="B13" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="32"/>
-      <c r="D13" s="32"/>
-      <c r="E13" s="32"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="32"/>
-      <c r="H13" s="32"/>
-      <c r="I13" s="32"/>
+      <c r="C13" s="50"/>
+      <c r="D13" s="50"/>
+      <c r="E13" s="50"/>
+      <c r="F13" s="50"/>
+      <c r="G13" s="50"/>
+      <c r="H13" s="50"/>
+      <c r="I13" s="50"/>
     </row>
     <row r="14" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="37"/>
+      <c r="A14" s="23"/>
       <c r="B14" s="7" t="s">
         <v>10</v>
       </c>
@@ -1300,7 +1313,7 @@
       <c r="I14" s="9"/>
     </row>
     <row r="15" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="37"/>
+      <c r="A15" s="24"/>
       <c r="B15" s="7" t="s">
         <v>11</v>
       </c>
@@ -1315,22 +1328,22 @@
       <c r="I15" s="9"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="37">
+      <c r="A16" s="18">
         <v>2</v>
       </c>
-      <c r="B16" s="41" t="s">
+      <c r="B16" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="42"/>
-      <c r="D16" s="42"/>
-      <c r="E16" s="42"/>
-      <c r="F16" s="43"/>
-      <c r="G16" s="43"/>
-      <c r="H16" s="43"/>
-      <c r="I16" s="44"/>
+      <c r="C16" s="55"/>
+      <c r="D16" s="55"/>
+      <c r="E16" s="55"/>
+      <c r="F16" s="56"/>
+      <c r="G16" s="56"/>
+      <c r="H16" s="56"/>
+      <c r="I16" s="57"/>
     </row>
     <row r="17" spans="1:9" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="37"/>
+      <c r="A17" s="20"/>
       <c r="B17" s="9" t="s">
         <v>10</v>
       </c>
@@ -1345,7 +1358,7 @@
       <c r="I17" s="9"/>
     </row>
     <row r="18" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="37"/>
+      <c r="A18" s="20"/>
       <c r="B18" s="9" t="s">
         <v>11</v>
       </c>
@@ -1360,7 +1373,7 @@
       <c r="I18" s="9"/>
     </row>
     <row r="19" spans="1:9" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="37"/>
+      <c r="A19" s="20"/>
       <c r="B19" s="9" t="s">
         <v>16</v>
       </c>
@@ -1375,7 +1388,7 @@
       <c r="I19" s="9"/>
     </row>
     <row r="20" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="37"/>
+      <c r="A20" s="19"/>
       <c r="B20" s="9" t="s">
         <v>17</v>
       </c>
@@ -1390,787 +1403,787 @@
       <c r="I20" s="9"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="37">
+      <c r="A21" s="18">
         <v>3</v>
       </c>
-      <c r="B21" s="32" t="s">
+      <c r="B21" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="32"/>
-      <c r="D21" s="32"/>
-      <c r="E21" s="32"/>
-      <c r="F21" s="33"/>
-      <c r="G21" s="33"/>
-      <c r="H21" s="33"/>
-      <c r="I21" s="33"/>
+      <c r="C21" s="50"/>
+      <c r="D21" s="50"/>
+      <c r="E21" s="50"/>
+      <c r="F21" s="51"/>
+      <c r="G21" s="51"/>
+      <c r="H21" s="51"/>
+      <c r="I21" s="51"/>
     </row>
     <row r="22" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="37"/>
+      <c r="A22" s="20"/>
       <c r="B22" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C22" s="29" t="s">
+      <c r="C22" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="D22" s="30"/>
-      <c r="E22" s="31"/>
+      <c r="D22" s="43"/>
+      <c r="E22" s="44"/>
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
       <c r="H22" s="9"/>
       <c r="I22" s="9"/>
     </row>
     <row r="23" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="37"/>
+      <c r="A23" s="20"/>
       <c r="B23" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="29" t="s">
+      <c r="C23" s="42" t="s">
         <v>48</v>
       </c>
-      <c r="D23" s="30"/>
-      <c r="E23" s="31"/>
+      <c r="D23" s="43"/>
+      <c r="E23" s="44"/>
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
       <c r="H23" s="9"/>
       <c r="I23" s="9"/>
     </row>
     <row r="24" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="37"/>
+      <c r="A24" s="20"/>
       <c r="B24" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C24" s="29" t="s">
+      <c r="C24" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="D24" s="30"/>
-      <c r="E24" s="31"/>
+      <c r="D24" s="43"/>
+      <c r="E24" s="44"/>
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
       <c r="H24" s="9"/>
       <c r="I24" s="9"/>
     </row>
     <row r="25" spans="1:9" s="3" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="37"/>
+      <c r="A25" s="20"/>
       <c r="B25" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="29" t="s">
+      <c r="C25" s="42" t="s">
         <v>68</v>
       </c>
-      <c r="D25" s="30"/>
-      <c r="E25" s="31"/>
+      <c r="D25" s="43"/>
+      <c r="E25" s="44"/>
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
       <c r="H25" s="9"/>
       <c r="I25" s="9"/>
     </row>
     <row r="26" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="37"/>
+      <c r="A26" s="20"/>
       <c r="B26" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C26" s="29" t="s">
+      <c r="C26" s="42" t="s">
         <v>69</v>
       </c>
-      <c r="D26" s="30"/>
-      <c r="E26" s="31"/>
+      <c r="D26" s="43"/>
+      <c r="E26" s="44"/>
       <c r="F26" s="9"/>
       <c r="G26" s="9"/>
       <c r="H26" s="9"/>
       <c r="I26" s="9"/>
     </row>
     <row r="27" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="37"/>
+      <c r="A27" s="19"/>
       <c r="B27" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C27" s="29" t="s">
+      <c r="C27" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="D27" s="30"/>
-      <c r="E27" s="31"/>
+      <c r="D27" s="43"/>
+      <c r="E27" s="44"/>
       <c r="F27" s="9"/>
       <c r="G27" s="9"/>
       <c r="H27" s="9"/>
       <c r="I27" s="9"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="15">
+      <c r="A28" s="18">
         <v>4</v>
       </c>
-      <c r="B28" s="41" t="s">
+      <c r="B28" s="54" t="s">
         <v>22</v>
       </c>
-      <c r="C28" s="42"/>
-      <c r="D28" s="42"/>
-      <c r="E28" s="42"/>
-      <c r="F28" s="43"/>
-      <c r="G28" s="43"/>
-      <c r="H28" s="43"/>
-      <c r="I28" s="44"/>
+      <c r="C28" s="55"/>
+      <c r="D28" s="55"/>
+      <c r="E28" s="55"/>
+      <c r="F28" s="56"/>
+      <c r="G28" s="56"/>
+      <c r="H28" s="56"/>
+      <c r="I28" s="57"/>
     </row>
     <row r="29" spans="1:9" s="3" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="23"/>
+      <c r="A29" s="20"/>
       <c r="B29" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C29" s="29" t="s">
+      <c r="C29" s="42" t="s">
         <v>70</v>
       </c>
-      <c r="D29" s="30"/>
-      <c r="E29" s="31"/>
+      <c r="D29" s="43"/>
+      <c r="E29" s="44"/>
       <c r="F29" s="9"/>
       <c r="G29" s="9"/>
       <c r="H29" s="9"/>
       <c r="I29" s="9"/>
     </row>
     <row r="30" spans="1:9" s="3" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="23"/>
+      <c r="A30" s="20"/>
       <c r="B30" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C30" s="29" t="s">
+      <c r="C30" s="42" t="s">
         <v>49</v>
       </c>
-      <c r="D30" s="30"/>
-      <c r="E30" s="31"/>
+      <c r="D30" s="43"/>
+      <c r="E30" s="44"/>
       <c r="F30" s="9"/>
       <c r="G30" s="9"/>
       <c r="H30" s="9"/>
       <c r="I30" s="9"/>
     </row>
     <row r="31" spans="1:9" s="3" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="22"/>
+      <c r="A31" s="20"/>
       <c r="B31" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C31" s="29" t="s">
+      <c r="C31" s="42" t="s">
         <v>71</v>
       </c>
-      <c r="D31" s="30"/>
-      <c r="E31" s="31"/>
+      <c r="D31" s="43"/>
+      <c r="E31" s="44"/>
       <c r="F31" s="9"/>
       <c r="G31" s="9"/>
       <c r="H31" s="9"/>
       <c r="I31" s="9"/>
     </row>
     <row r="32" spans="1:9" s="3" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="21"/>
+      <c r="A32" s="20"/>
       <c r="B32" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C32" s="29" t="s">
+      <c r="C32" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="D32" s="30"/>
-      <c r="E32" s="31"/>
+      <c r="D32" s="43"/>
+      <c r="E32" s="44"/>
       <c r="F32" s="9"/>
       <c r="G32" s="9"/>
       <c r="H32" s="9"/>
       <c r="I32" s="9"/>
     </row>
     <row r="33" spans="1:9" s="3" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="22"/>
+      <c r="A33" s="19"/>
       <c r="B33" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C33" s="29" t="s">
+      <c r="C33" s="42" t="s">
         <v>72</v>
       </c>
-      <c r="D33" s="30"/>
-      <c r="E33" s="31"/>
+      <c r="D33" s="43"/>
+      <c r="E33" s="44"/>
       <c r="F33" s="9"/>
       <c r="G33" s="9"/>
       <c r="H33" s="9"/>
       <c r="I33" s="9"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A34" s="21">
+      <c r="A34" s="18">
         <v>5</v>
       </c>
-      <c r="B34" s="32" t="s">
+      <c r="B34" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="C34" s="32"/>
-      <c r="D34" s="32"/>
-      <c r="E34" s="32"/>
-      <c r="F34" s="33"/>
-      <c r="G34" s="33"/>
-      <c r="H34" s="33"/>
-      <c r="I34" s="33"/>
+      <c r="C34" s="50"/>
+      <c r="D34" s="50"/>
+      <c r="E34" s="50"/>
+      <c r="F34" s="51"/>
+      <c r="G34" s="51"/>
+      <c r="H34" s="51"/>
+      <c r="I34" s="51"/>
     </row>
     <row r="35" spans="1:9" s="3" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="22"/>
+      <c r="A35" s="20"/>
       <c r="B35" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C35" s="29" t="s">
+      <c r="C35" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="D35" s="30"/>
-      <c r="E35" s="31"/>
+      <c r="D35" s="43"/>
+      <c r="E35" s="44"/>
       <c r="F35" s="9"/>
       <c r="G35" s="9"/>
       <c r="H35" s="9"/>
       <c r="I35" s="9"/>
     </row>
     <row r="36" spans="1:9" s="3" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="53"/>
+      <c r="A36" s="20"/>
       <c r="B36" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C36" s="29" t="s">
+      <c r="C36" s="42" t="s">
         <v>73</v>
       </c>
-      <c r="D36" s="30"/>
-      <c r="E36" s="31"/>
+      <c r="D36" s="43"/>
+      <c r="E36" s="44"/>
       <c r="F36" s="9"/>
       <c r="G36" s="9"/>
       <c r="H36" s="9"/>
       <c r="I36" s="9"/>
     </row>
     <row r="37" spans="1:9" s="3" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="54"/>
+      <c r="A37" s="20"/>
       <c r="B37" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C37" s="29" t="s">
+      <c r="C37" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="D37" s="30"/>
-      <c r="E37" s="31"/>
+      <c r="D37" s="43"/>
+      <c r="E37" s="44"/>
       <c r="F37" s="9"/>
       <c r="G37" s="9"/>
       <c r="H37" s="9"/>
       <c r="I37" s="9"/>
     </row>
     <row r="38" spans="1:9" s="3" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="55"/>
+      <c r="A38" s="19"/>
       <c r="B38" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C38" s="29" t="s">
+      <c r="C38" s="42" t="s">
         <v>74</v>
       </c>
-      <c r="D38" s="30"/>
-      <c r="E38" s="31"/>
+      <c r="D38" s="43"/>
+      <c r="E38" s="44"/>
       <c r="F38" s="9"/>
       <c r="G38" s="9"/>
       <c r="H38" s="9"/>
       <c r="I38" s="9"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A39" s="37">
+      <c r="A39" s="18">
         <v>6</v>
       </c>
-      <c r="B39" s="32" t="s">
+      <c r="B39" s="50" t="s">
         <v>24</v>
       </c>
-      <c r="C39" s="32"/>
-      <c r="D39" s="32"/>
-      <c r="E39" s="32"/>
-      <c r="F39" s="33"/>
-      <c r="G39" s="33"/>
-      <c r="H39" s="33"/>
-      <c r="I39" s="33"/>
+      <c r="C39" s="50"/>
+      <c r="D39" s="50"/>
+      <c r="E39" s="50"/>
+      <c r="F39" s="51"/>
+      <c r="G39" s="51"/>
+      <c r="H39" s="51"/>
+      <c r="I39" s="51"/>
     </row>
     <row r="40" spans="1:9" s="3" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="37"/>
+      <c r="A40" s="20"/>
       <c r="B40" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C40" s="29" t="s">
+      <c r="C40" s="42" t="s">
         <v>53</v>
       </c>
-      <c r="D40" s="30"/>
-      <c r="E40" s="31"/>
+      <c r="D40" s="43"/>
+      <c r="E40" s="44"/>
       <c r="F40" s="9"/>
       <c r="G40" s="9"/>
       <c r="H40" s="9"/>
       <c r="I40" s="9"/>
     </row>
     <row r="41" spans="1:9" s="3" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="37"/>
+      <c r="A41" s="20"/>
       <c r="B41" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C41" s="29" t="s">
+      <c r="C41" s="42" t="s">
         <v>75</v>
       </c>
-      <c r="D41" s="30"/>
-      <c r="E41" s="31"/>
+      <c r="D41" s="43"/>
+      <c r="E41" s="44"/>
       <c r="F41" s="9"/>
       <c r="G41" s="9"/>
       <c r="H41" s="9"/>
       <c r="I41" s="9"/>
     </row>
     <row r="42" spans="1:9" s="3" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="37"/>
+      <c r="A42" s="20"/>
       <c r="B42" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C42" s="29" t="s">
+      <c r="C42" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="D42" s="30"/>
-      <c r="E42" s="31"/>
+      <c r="D42" s="43"/>
+      <c r="E42" s="44"/>
       <c r="F42" s="9"/>
       <c r="G42" s="9"/>
       <c r="H42" s="9"/>
       <c r="I42" s="9"/>
     </row>
     <row r="43" spans="1:9" s="3" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="37"/>
+      <c r="A43" s="19"/>
       <c r="B43" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C43" s="29" t="s">
+      <c r="C43" s="42" t="s">
         <v>76</v>
       </c>
-      <c r="D43" s="30"/>
-      <c r="E43" s="31"/>
+      <c r="D43" s="43"/>
+      <c r="E43" s="44"/>
       <c r="F43" s="9"/>
       <c r="G43" s="9"/>
       <c r="H43" s="9"/>
       <c r="I43" s="9"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A44" s="37">
+      <c r="A44" s="18">
         <v>7</v>
       </c>
-      <c r="B44" s="32" t="s">
+      <c r="B44" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="C44" s="32"/>
-      <c r="D44" s="32"/>
-      <c r="E44" s="32"/>
-      <c r="F44" s="33"/>
-      <c r="G44" s="33"/>
-      <c r="H44" s="33"/>
-      <c r="I44" s="33"/>
+      <c r="C44" s="50"/>
+      <c r="D44" s="50"/>
+      <c r="E44" s="50"/>
+      <c r="F44" s="51"/>
+      <c r="G44" s="51"/>
+      <c r="H44" s="51"/>
+      <c r="I44" s="51"/>
     </row>
     <row r="45" spans="1:9" s="3" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="37"/>
+      <c r="A45" s="20"/>
       <c r="B45" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C45" s="29" t="s">
+      <c r="C45" s="42" t="s">
         <v>77</v>
       </c>
-      <c r="D45" s="30"/>
-      <c r="E45" s="31"/>
+      <c r="D45" s="43"/>
+      <c r="E45" s="44"/>
       <c r="F45" s="9"/>
       <c r="G45" s="9"/>
       <c r="H45" s="9"/>
       <c r="I45" s="9"/>
     </row>
     <row r="46" spans="1:9" s="3" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="37"/>
+      <c r="A46" s="19"/>
       <c r="B46" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C46" s="29" t="s">
+      <c r="C46" s="42" t="s">
         <v>78</v>
       </c>
-      <c r="D46" s="30"/>
-      <c r="E46" s="31"/>
+      <c r="D46" s="43"/>
+      <c r="E46" s="44"/>
       <c r="F46" s="9"/>
       <c r="G46" s="9"/>
       <c r="H46" s="9"/>
       <c r="I46" s="9"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A47" s="21">
+      <c r="A47" s="18">
         <v>8</v>
       </c>
-      <c r="B47" s="32" t="s">
+      <c r="B47" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="C47" s="32"/>
-      <c r="D47" s="32"/>
-      <c r="E47" s="32"/>
-      <c r="F47" s="33"/>
-      <c r="G47" s="33"/>
-      <c r="H47" s="33"/>
-      <c r="I47" s="33"/>
+      <c r="C47" s="50"/>
+      <c r="D47" s="50"/>
+      <c r="E47" s="50"/>
+      <c r="F47" s="51"/>
+      <c r="G47" s="51"/>
+      <c r="H47" s="51"/>
+      <c r="I47" s="51"/>
     </row>
     <row r="48" spans="1:9" s="3" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="23"/>
+      <c r="A48" s="20"/>
       <c r="B48" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C48" s="29" t="s">
+      <c r="C48" s="42" t="s">
         <v>79</v>
       </c>
-      <c r="D48" s="30"/>
-      <c r="E48" s="31"/>
+      <c r="D48" s="43"/>
+      <c r="E48" s="44"/>
       <c r="F48" s="9"/>
       <c r="G48" s="9"/>
       <c r="H48" s="9"/>
       <c r="I48" s="9"/>
     </row>
     <row r="49" spans="1:9" s="3" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="23"/>
+      <c r="A49" s="20"/>
       <c r="B49" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C49" s="29" t="s">
+      <c r="C49" s="42" t="s">
         <v>55</v>
       </c>
-      <c r="D49" s="30"/>
-      <c r="E49" s="31"/>
+      <c r="D49" s="43"/>
+      <c r="E49" s="44"/>
       <c r="F49" s="9"/>
       <c r="G49" s="9"/>
       <c r="H49" s="9"/>
       <c r="I49" s="9"/>
     </row>
     <row r="50" spans="1:9" s="3" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="23"/>
+      <c r="A50" s="20"/>
       <c r="B50" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C50" s="29" t="s">
+      <c r="C50" s="42" t="s">
         <v>103</v>
       </c>
-      <c r="D50" s="30"/>
-      <c r="E50" s="31"/>
+      <c r="D50" s="43"/>
+      <c r="E50" s="44"/>
       <c r="F50" s="9"/>
       <c r="G50" s="9"/>
       <c r="H50" s="9"/>
       <c r="I50" s="9"/>
     </row>
     <row r="51" spans="1:9" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="23"/>
+      <c r="A51" s="20"/>
       <c r="B51" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C51" s="29" t="s">
+      <c r="C51" s="42" t="s">
         <v>80</v>
       </c>
-      <c r="D51" s="30"/>
-      <c r="E51" s="31"/>
+      <c r="D51" s="43"/>
+      <c r="E51" s="44"/>
       <c r="F51" s="9"/>
       <c r="G51" s="9"/>
       <c r="H51" s="9"/>
       <c r="I51" s="9"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A52" s="23"/>
-      <c r="B52" s="21" t="s">
+      <c r="A52" s="20"/>
+      <c r="B52" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="C52" s="24" t="s">
+      <c r="C52" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="D52" s="25"/>
-      <c r="E52" s="26"/>
+      <c r="D52" s="62"/>
+      <c r="E52" s="49"/>
       <c r="F52" s="9"/>
       <c r="G52" s="9"/>
       <c r="H52" s="9"/>
       <c r="I52" s="9"/>
     </row>
     <row r="53" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="23"/>
-      <c r="B53" s="23"/>
-      <c r="C53" s="16" t="s">
+      <c r="A53" s="20"/>
+      <c r="B53" s="28"/>
+      <c r="C53" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="D53" s="29" t="s">
+      <c r="D53" s="42" t="s">
         <v>81</v>
       </c>
-      <c r="E53" s="31"/>
+      <c r="E53" s="44"/>
       <c r="F53" s="9"/>
       <c r="G53" s="9"/>
       <c r="H53" s="9"/>
       <c r="I53" s="9"/>
     </row>
     <row r="54" spans="1:9" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="23"/>
-      <c r="B54" s="23"/>
-      <c r="C54" s="17" t="s">
+      <c r="A54" s="20"/>
+      <c r="B54" s="28"/>
+      <c r="C54" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="D54" s="29" t="s">
+      <c r="D54" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="E54" s="31"/>
+      <c r="E54" s="44"/>
       <c r="F54" s="9"/>
       <c r="G54" s="9"/>
       <c r="H54" s="9"/>
       <c r="I54" s="9"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A55" s="23"/>
-      <c r="B55" s="23"/>
-      <c r="C55" s="17" t="s">
+      <c r="A55" s="20"/>
+      <c r="B55" s="28"/>
+      <c r="C55" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="D55" s="24" t="s">
+      <c r="D55" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="E55" s="26"/>
+      <c r="E55" s="49"/>
       <c r="F55" s="9"/>
       <c r="G55" s="9"/>
       <c r="H55" s="9"/>
       <c r="I55" s="9"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A56" s="23"/>
-      <c r="B56" s="23"/>
-      <c r="C56" s="17" t="s">
+      <c r="A56" s="20"/>
+      <c r="B56" s="28"/>
+      <c r="C56" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="D56" s="24" t="s">
+      <c r="D56" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="E56" s="26"/>
+      <c r="E56" s="49"/>
       <c r="F56" s="9"/>
       <c r="G56" s="9"/>
       <c r="H56" s="9"/>
       <c r="I56" s="9"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A57" s="23"/>
-      <c r="B57" s="23"/>
-      <c r="C57" s="17" t="s">
+      <c r="A57" s="20"/>
+      <c r="B57" s="28"/>
+      <c r="C57" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="D57" s="24" t="s">
+      <c r="D57" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="E57" s="26"/>
+      <c r="E57" s="49"/>
       <c r="F57" s="9"/>
       <c r="G57" s="9"/>
       <c r="H57" s="9"/>
       <c r="I57" s="9"/>
     </row>
     <row r="58" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="23"/>
-      <c r="B58" s="23"/>
-      <c r="C58" s="17" t="s">
+      <c r="A58" s="20"/>
+      <c r="B58" s="28"/>
+      <c r="C58" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="D58" s="29" t="s">
+      <c r="D58" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="E58" s="31"/>
+      <c r="E58" s="44"/>
       <c r="F58" s="9"/>
       <c r="G58" s="9"/>
       <c r="H58" s="9"/>
       <c r="I58" s="9"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A59" s="23"/>
-      <c r="B59" s="23"/>
-      <c r="C59" s="17" t="s">
+      <c r="A59" s="20"/>
+      <c r="B59" s="28"/>
+      <c r="C59" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="D59" s="24" t="s">
+      <c r="D59" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="E59" s="26"/>
+      <c r="E59" s="49"/>
       <c r="F59" s="9"/>
       <c r="G59" s="9"/>
       <c r="H59" s="9"/>
       <c r="I59" s="9"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A60" s="23"/>
-      <c r="B60" s="23"/>
-      <c r="C60" s="17" t="s">
+      <c r="A60" s="20"/>
+      <c r="B60" s="28"/>
+      <c r="C60" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="D60" s="24" t="s">
+      <c r="D60" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="E60" s="26"/>
+      <c r="E60" s="49"/>
       <c r="F60" s="9"/>
       <c r="G60" s="9"/>
       <c r="H60" s="9"/>
       <c r="I60" s="9"/>
     </row>
     <row r="61" spans="1:9" ht="69.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="23"/>
-      <c r="B61" s="23"/>
-      <c r="C61" s="17" t="s">
+      <c r="A61" s="20"/>
+      <c r="B61" s="28"/>
+      <c r="C61" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="D61" s="29" t="s">
+      <c r="D61" s="42" t="s">
         <v>82</v>
       </c>
-      <c r="E61" s="31"/>
+      <c r="E61" s="44"/>
       <c r="F61" s="9"/>
       <c r="G61" s="9"/>
       <c r="H61" s="9"/>
       <c r="I61" s="9"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A62" s="23"/>
-      <c r="B62" s="23"/>
-      <c r="C62" s="17" t="s">
+      <c r="A62" s="20"/>
+      <c r="B62" s="28"/>
+      <c r="C62" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="D62" s="24" t="s">
+      <c r="D62" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="E62" s="26"/>
+      <c r="E62" s="49"/>
       <c r="F62" s="9"/>
       <c r="G62" s="9"/>
       <c r="H62" s="9"/>
       <c r="I62" s="9"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A63" s="23"/>
-      <c r="B63" s="22"/>
-      <c r="C63" s="17" t="s">
+      <c r="A63" s="20"/>
+      <c r="B63" s="29"/>
+      <c r="C63" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="D63" s="24" t="s">
+      <c r="D63" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="E63" s="26"/>
+      <c r="E63" s="49"/>
       <c r="F63" s="9"/>
       <c r="G63" s="9"/>
       <c r="H63" s="9"/>
       <c r="I63" s="9"/>
     </row>
     <row r="64" spans="1:9" s="3" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="22"/>
+      <c r="A64" s="20"/>
       <c r="B64" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C64" s="29" t="s">
+      <c r="C64" s="42" t="s">
         <v>83</v>
       </c>
-      <c r="D64" s="30"/>
-      <c r="E64" s="31"/>
+      <c r="D64" s="43"/>
+      <c r="E64" s="44"/>
       <c r="F64" s="9"/>
       <c r="G64" s="9"/>
       <c r="H64" s="9"/>
       <c r="I64" s="9"/>
     </row>
     <row r="65" spans="1:9" s="3" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="52"/>
+      <c r="A65" s="19"/>
       <c r="B65" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="C65" s="29" t="s">
+      <c r="C65" s="42" t="s">
         <v>84</v>
       </c>
-      <c r="D65" s="30"/>
-      <c r="E65" s="31"/>
+      <c r="D65" s="43"/>
+      <c r="E65" s="44"/>
       <c r="F65" s="9"/>
       <c r="G65" s="9"/>
       <c r="H65" s="9"/>
       <c r="I65" s="9"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A66" s="37">
+      <c r="A66" s="18">
         <v>9</v>
       </c>
-      <c r="B66" s="32" t="s">
+      <c r="B66" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="C66" s="32"/>
-      <c r="D66" s="32"/>
-      <c r="E66" s="32"/>
-      <c r="F66" s="33"/>
-      <c r="G66" s="33"/>
-      <c r="H66" s="33"/>
-      <c r="I66" s="33"/>
+      <c r="C66" s="50"/>
+      <c r="D66" s="50"/>
+      <c r="E66" s="50"/>
+      <c r="F66" s="51"/>
+      <c r="G66" s="51"/>
+      <c r="H66" s="51"/>
+      <c r="I66" s="51"/>
     </row>
     <row r="67" spans="1:9" s="3" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="37"/>
+      <c r="A67" s="20"/>
       <c r="B67" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C67" s="29" t="s">
+      <c r="C67" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="D67" s="30"/>
-      <c r="E67" s="31"/>
+      <c r="D67" s="43"/>
+      <c r="E67" s="44"/>
       <c r="F67" s="9"/>
       <c r="G67" s="9"/>
       <c r="H67" s="9"/>
       <c r="I67" s="9"/>
     </row>
     <row r="68" spans="1:9" s="3" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="37"/>
+      <c r="A68" s="20"/>
       <c r="B68" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C68" s="29" t="s">
+      <c r="C68" s="42" t="s">
         <v>85</v>
       </c>
-      <c r="D68" s="30"/>
-      <c r="E68" s="31"/>
+      <c r="D68" s="43"/>
+      <c r="E68" s="44"/>
       <c r="F68" s="9"/>
       <c r="G68" s="9"/>
       <c r="H68" s="9"/>
       <c r="I68" s="9"/>
     </row>
     <row r="69" spans="1:9" s="3" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="37"/>
+      <c r="A69" s="20"/>
       <c r="B69" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C69" s="29" t="s">
+      <c r="C69" s="42" t="s">
         <v>104</v>
       </c>
-      <c r="D69" s="30"/>
-      <c r="E69" s="31"/>
+      <c r="D69" s="43"/>
+      <c r="E69" s="44"/>
       <c r="F69" s="9"/>
       <c r="G69" s="9"/>
       <c r="H69" s="9"/>
       <c r="I69" s="9"/>
     </row>
     <row r="70" spans="1:9" s="3" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="37"/>
+      <c r="A70" s="20"/>
       <c r="B70" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C70" s="29" t="s">
+      <c r="C70" s="42" t="s">
         <v>86</v>
       </c>
-      <c r="D70" s="30"/>
-      <c r="E70" s="31"/>
+      <c r="D70" s="43"/>
+      <c r="E70" s="44"/>
       <c r="F70" s="9"/>
       <c r="G70" s="9"/>
       <c r="H70" s="9"/>
       <c r="I70" s="9"/>
     </row>
     <row r="71" spans="1:9" s="3" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="37"/>
+      <c r="A71" s="19"/>
       <c r="B71" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C71" s="29" t="s">
+      <c r="C71" s="42" t="s">
         <v>57</v>
       </c>
-      <c r="D71" s="30"/>
-      <c r="E71" s="31"/>
+      <c r="D71" s="43"/>
+      <c r="E71" s="44"/>
       <c r="F71" s="9"/>
       <c r="G71" s="9"/>
       <c r="H71" s="9"/>
       <c r="I71" s="9"/>
     </row>
     <row r="72" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="37">
+      <c r="A72" s="18">
         <v>10</v>
       </c>
-      <c r="B72" s="33" t="s">
+      <c r="B72" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="C72" s="33"/>
-      <c r="D72" s="33"/>
-      <c r="E72" s="33"/>
-      <c r="F72" s="33"/>
-      <c r="G72" s="33"/>
-      <c r="H72" s="33"/>
-      <c r="I72" s="33"/>
+      <c r="C72" s="51"/>
+      <c r="D72" s="51"/>
+      <c r="E72" s="51"/>
+      <c r="F72" s="51"/>
+      <c r="G72" s="51"/>
+      <c r="H72" s="51"/>
+      <c r="I72" s="51"/>
     </row>
     <row r="73" spans="1:9" s="4" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="37"/>
+      <c r="A73" s="20"/>
       <c r="B73" s="9" t="s">
         <v>10</v>
       </c>
@@ -2185,7 +2198,7 @@
       <c r="I73" s="9"/>
     </row>
     <row r="74" spans="1:9" s="4" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="37"/>
+      <c r="A74" s="20"/>
       <c r="B74" s="9" t="s">
         <v>11</v>
       </c>
@@ -2200,7 +2213,7 @@
       <c r="I74" s="9"/>
     </row>
     <row r="75" spans="1:9" s="4" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="37"/>
+      <c r="A75" s="20"/>
       <c r="B75" s="9" t="s">
         <v>16</v>
       </c>
@@ -2215,7 +2228,7 @@
       <c r="I75" s="9"/>
     </row>
     <row r="76" spans="1:9" s="4" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="37"/>
+      <c r="A76" s="20"/>
       <c r="B76" s="9" t="s">
         <v>17</v>
       </c>
@@ -2230,7 +2243,7 @@
       <c r="I76" s="9"/>
     </row>
     <row r="77" spans="1:9" s="4" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="37"/>
+      <c r="A77" s="20"/>
       <c r="B77" s="9" t="s">
         <v>19</v>
       </c>
@@ -2245,7 +2258,7 @@
       <c r="I77" s="9"/>
     </row>
     <row r="78" spans="1:9" s="4" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="37"/>
+      <c r="A78" s="19"/>
       <c r="B78" s="9" t="s">
         <v>20</v>
       </c>
@@ -2260,67 +2273,67 @@
       <c r="I78" s="9"/>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A79" s="37">
+      <c r="A79" s="18">
         <v>11</v>
       </c>
-      <c r="B79" s="32" t="s">
+      <c r="B79" s="50" t="s">
         <v>41</v>
       </c>
-      <c r="C79" s="32"/>
-      <c r="D79" s="32"/>
-      <c r="E79" s="32"/>
-      <c r="F79" s="33"/>
-      <c r="G79" s="33"/>
-      <c r="H79" s="33"/>
-      <c r="I79" s="33"/>
+      <c r="C79" s="50"/>
+      <c r="D79" s="50"/>
+      <c r="E79" s="50"/>
+      <c r="F79" s="51"/>
+      <c r="G79" s="51"/>
+      <c r="H79" s="51"/>
+      <c r="I79" s="51"/>
     </row>
     <row r="80" spans="1:9" s="3" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="37"/>
+      <c r="A80" s="20"/>
       <c r="B80" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C80" s="29" t="s">
+      <c r="C80" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="D80" s="30"/>
-      <c r="E80" s="31"/>
+      <c r="D80" s="43"/>
+      <c r="E80" s="44"/>
       <c r="F80" s="9"/>
       <c r="G80" s="9"/>
       <c r="H80" s="9"/>
       <c r="I80" s="9"/>
     </row>
     <row r="81" spans="1:9" s="3" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="37"/>
+      <c r="A81" s="19"/>
       <c r="B81" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C81" s="29" t="s">
+      <c r="C81" s="42" t="s">
         <v>90</v>
       </c>
-      <c r="D81" s="30"/>
-      <c r="E81" s="31"/>
+      <c r="D81" s="43"/>
+      <c r="E81" s="44"/>
       <c r="F81" s="9"/>
       <c r="G81" s="9"/>
       <c r="H81" s="9"/>
       <c r="I81" s="9"/>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A82" s="37">
+      <c r="A82" s="18">
         <v>12</v>
       </c>
-      <c r="B82" s="32" t="s">
+      <c r="B82" s="50" t="s">
         <v>42</v>
       </c>
-      <c r="C82" s="32"/>
-      <c r="D82" s="32"/>
-      <c r="E82" s="32"/>
-      <c r="F82" s="33"/>
-      <c r="G82" s="33"/>
-      <c r="H82" s="33"/>
-      <c r="I82" s="33"/>
+      <c r="C82" s="50"/>
+      <c r="D82" s="50"/>
+      <c r="E82" s="50"/>
+      <c r="F82" s="51"/>
+      <c r="G82" s="51"/>
+      <c r="H82" s="51"/>
+      <c r="I82" s="51"/>
     </row>
     <row r="83" spans="1:9" s="4" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="37"/>
+      <c r="A83" s="20"/>
       <c r="B83" s="9" t="s">
         <v>10</v>
       </c>
@@ -2335,7 +2348,7 @@
       <c r="I83" s="9"/>
     </row>
     <row r="84" spans="1:9" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="37"/>
+      <c r="A84" s="20"/>
       <c r="B84" s="9" t="s">
         <v>11</v>
       </c>
@@ -2350,7 +2363,7 @@
       <c r="I84" s="9"/>
     </row>
     <row r="85" spans="1:9" s="4" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="37"/>
+      <c r="A85" s="20"/>
       <c r="B85" s="9" t="s">
         <v>16</v>
       </c>
@@ -2365,7 +2378,7 @@
       <c r="I85" s="9"/>
     </row>
     <row r="86" spans="1:9" s="4" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="37"/>
+      <c r="A86" s="19"/>
       <c r="B86" s="9" t="s">
         <v>17</v>
       </c>
@@ -2381,187 +2394,264 @@
     </row>
     <row r="87" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="8"/>
-      <c r="B87" s="39" t="s">
+      <c r="B87" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="C87" s="39"/>
-      <c r="D87" s="39"/>
+      <c r="C87" s="53"/>
+      <c r="D87" s="53"/>
       <c r="E87" s="10"/>
       <c r="F87" s="13"/>
       <c r="G87" s="13"/>
     </row>
     <row r="88" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="8"/>
-      <c r="B88" s="39" t="s">
+      <c r="B88" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="C88" s="39"/>
-      <c r="D88" s="39"/>
+      <c r="C88" s="53"/>
+      <c r="D88" s="53"/>
       <c r="E88" s="10"/>
-      <c r="F88" s="40"/>
-      <c r="G88" s="40"/>
-    </row>
-    <row r="94" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="F88" s="33"/>
+      <c r="G88" s="33"/>
+    </row>
+    <row r="93" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="94" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A94" s="38" t="s">
+        <v>94</v>
+      </c>
+      <c r="B94" s="38"/>
+      <c r="C94" s="38"/>
+      <c r="D94" s="41" t="s">
+        <v>112</v>
+      </c>
+      <c r="E94" s="41"/>
+      <c r="F94" s="41"/>
+      <c r="G94" s="39" t="s">
+        <v>95</v>
+      </c>
+    </row>
     <row r="95" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="58" t="s">
-        <v>94</v>
-      </c>
-      <c r="B95" s="58"/>
-      <c r="C95" s="58"/>
-      <c r="D95" s="51" t="s">
-        <v>112</v>
-      </c>
-      <c r="E95" s="51"/>
-      <c r="F95" s="51"/>
-      <c r="G95" s="50" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="96" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="58"/>
-      <c r="B96" s="58"/>
-      <c r="C96" s="58"/>
-      <c r="D96" s="57" t="s">
+      <c r="A95" s="38"/>
+      <c r="B95" s="38"/>
+      <c r="C95" s="38"/>
+      <c r="D95" s="40" t="s">
         <v>113</v>
       </c>
-      <c r="E96" s="57"/>
-      <c r="F96" s="57"/>
-      <c r="G96" s="50"/>
-    </row>
-    <row r="97" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="98" spans="1:9" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B98" s="49" t="s">
+      <c r="E95" s="40"/>
+      <c r="F95" s="40"/>
+      <c r="G95" s="39"/>
+    </row>
+    <row r="96" spans="1:9" s="17" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A96" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="B96" s="26"/>
+      <c r="C96" s="26"/>
+      <c r="D96" s="25"/>
+      <c r="E96" s="25"/>
+      <c r="F96" s="25"/>
+      <c r="G96" s="22"/>
+    </row>
+    <row r="97" spans="1:9" s="17" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A97" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="B97" s="26"/>
+      <c r="C97" s="26"/>
+      <c r="D97" s="25"/>
+      <c r="E97" s="25"/>
+      <c r="F97" s="25"/>
+      <c r="G97" s="22"/>
+    </row>
+    <row r="98" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A98" s="26" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B99" s="37" t="s">
         <v>96</v>
       </c>
-      <c r="C98" s="49"/>
-      <c r="D98" s="49"/>
-      <c r="E98" s="49"/>
-      <c r="F98" s="49"/>
-      <c r="G98" s="49"/>
-      <c r="H98" s="49"/>
-      <c r="I98" s="49"/>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B100" s="1" t="s">
+      <c r="C99" s="37"/>
+      <c r="D99" s="37"/>
+      <c r="E99" s="37"/>
+      <c r="F99" s="37"/>
+      <c r="G99" s="37"/>
+      <c r="H99" s="37"/>
+      <c r="I99" s="37"/>
+    </row>
+    <row r="100" spans="1:9" s="17" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B100" s="21"/>
+      <c r="C100" s="21"/>
+      <c r="D100" s="21"/>
+      <c r="E100" s="21"/>
+      <c r="F100" s="21"/>
+      <c r="G100" s="21"/>
+      <c r="H100" s="21"/>
+      <c r="I100" s="21"/>
+    </row>
+    <row r="101" spans="1:9" s="17" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A101" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="B101" s="21"/>
+      <c r="C101" s="21"/>
+      <c r="D101" s="21"/>
+      <c r="E101" s="21"/>
+      <c r="F101" s="21"/>
+      <c r="G101" s="21"/>
+      <c r="H101" s="21"/>
+      <c r="I101" s="21"/>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B103" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="E100" s="48" t="s">
+      <c r="E103" s="32" t="s">
         <v>99</v>
       </c>
-      <c r="F100" s="40" t="s">
+      <c r="F103" s="33" t="s">
         <v>105</v>
       </c>
-      <c r="G100" s="40"/>
-      <c r="H100" s="40" t="s">
+      <c r="G103" s="33"/>
+      <c r="H103" s="33" t="s">
         <v>106</v>
       </c>
-      <c r="I100" s="40"/>
-    </row>
-    <row r="101" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B101" s="19" t="s">
+      <c r="I103" s="33"/>
+    </row>
+    <row r="104" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B104" s="60" t="s">
         <v>98</v>
       </c>
-      <c r="C101" s="19"/>
-      <c r="D101" s="20"/>
-      <c r="E101" s="48"/>
-      <c r="F101" s="9" t="s">
+      <c r="C104" s="60"/>
+      <c r="D104" s="61"/>
+      <c r="E104" s="32"/>
+      <c r="F104" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="G101" s="12" t="s">
+      <c r="G104" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="H101" s="9" t="s">
+      <c r="H104" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="I101" s="12" t="s">
+      <c r="I104" s="12" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="102" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E102" s="48"/>
-      <c r="F102" s="11"/>
-      <c r="G102" s="11"/>
-      <c r="H102" s="8"/>
-      <c r="I102" s="8"/>
-    </row>
-    <row r="103" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E103" s="48"/>
-      <c r="F103" s="11"/>
-      <c r="G103" s="11"/>
-      <c r="H103" s="8"/>
-      <c r="I103" s="8"/>
-    </row>
-    <row r="104" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B106" s="1" t="s">
+    <row r="105" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E105" s="32"/>
+      <c r="F105" s="11"/>
+      <c r="G105" s="11"/>
+      <c r="H105" s="8"/>
+      <c r="I105" s="8"/>
+    </row>
+    <row r="106" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E106" s="32"/>
+      <c r="F106" s="11"/>
+      <c r="G106" s="11"/>
+      <c r="H106" s="8"/>
+      <c r="I106" s="8"/>
+    </row>
+    <row r="107" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B109" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="D106" s="14" t="s">
+      <c r="D109" s="14" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A110" s="18" t="s">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A113" s="59" t="s">
         <v>109</v>
       </c>
-      <c r="B110" s="18"/>
-      <c r="C110" s="18"/>
-      <c r="D110" s="18"/>
-      <c r="E110" s="18"/>
-      <c r="F110" s="18"/>
-    </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A111" s="18" t="s">
+      <c r="B113" s="59"/>
+      <c r="C113" s="59"/>
+      <c r="D113" s="59"/>
+      <c r="E113" s="59"/>
+      <c r="F113" s="59"/>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A114" s="59" t="s">
         <v>107</v>
       </c>
-      <c r="B111" s="18"/>
-      <c r="C111" s="18"/>
-      <c r="D111" s="18"/>
-      <c r="E111" s="18"/>
-      <c r="F111" s="18"/>
-    </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A112" s="18" t="s">
+      <c r="B114" s="59"/>
+      <c r="C114" s="59"/>
+      <c r="D114" s="59"/>
+      <c r="E114" s="59"/>
+      <c r="F114" s="59"/>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A115" s="59" t="s">
         <v>108</v>
       </c>
-      <c r="B112" s="18"/>
-      <c r="C112" s="18"/>
-      <c r="D112" s="18"/>
-      <c r="E112" s="18"/>
-      <c r="F112" s="18"/>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A113" s="18"/>
-      <c r="B113" s="18"/>
-      <c r="C113" s="18"/>
-      <c r="D113" s="18"/>
-      <c r="E113" s="18"/>
-      <c r="F113" s="18"/>
+      <c r="B115" s="59"/>
+      <c r="C115" s="59"/>
+      <c r="D115" s="59"/>
+      <c r="E115" s="59"/>
+      <c r="F115" s="59"/>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A116" s="59"/>
+      <c r="B116" s="59"/>
+      <c r="C116" s="59"/>
+      <c r="D116" s="59"/>
+      <c r="E116" s="59"/>
+      <c r="F116" s="59"/>
     </row>
   </sheetData>
-  <mergeCells count="115">
-    <mergeCell ref="A47:A64"/>
-    <mergeCell ref="D6:I6"/>
-    <mergeCell ref="D7:I7"/>
-    <mergeCell ref="D8:I8"/>
-    <mergeCell ref="D9:I9"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="E100:E103"/>
-    <mergeCell ref="F100:G100"/>
-    <mergeCell ref="H100:I100"/>
-    <mergeCell ref="C83:E83"/>
-    <mergeCell ref="C84:E84"/>
-    <mergeCell ref="C85:E85"/>
-    <mergeCell ref="C86:E86"/>
-    <mergeCell ref="B98:I98"/>
-    <mergeCell ref="A95:C96"/>
-    <mergeCell ref="G95:G96"/>
-    <mergeCell ref="D96:F96"/>
-    <mergeCell ref="D95:F95"/>
+  <mergeCells count="102">
+    <mergeCell ref="A113:F113"/>
+    <mergeCell ref="A114:F114"/>
+    <mergeCell ref="A115:F115"/>
+    <mergeCell ref="A116:F116"/>
+    <mergeCell ref="B104:D104"/>
+    <mergeCell ref="C52:E52"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="B52:B63"/>
+    <mergeCell ref="C42:E42"/>
+    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="C45:E45"/>
+    <mergeCell ref="C46:E46"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="C48:E48"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="B21:I21"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="B88:D88"/>
+    <mergeCell ref="F88:G88"/>
+    <mergeCell ref="B16:I16"/>
+    <mergeCell ref="B28:I28"/>
+    <mergeCell ref="B47:I47"/>
+    <mergeCell ref="B66:I66"/>
+    <mergeCell ref="B72:I72"/>
+    <mergeCell ref="B79:I79"/>
+    <mergeCell ref="B82:I82"/>
+    <mergeCell ref="B87:D87"/>
+    <mergeCell ref="B13:I13"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="C33:E33"/>
+    <mergeCell ref="C35:E35"/>
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="B34:I34"/>
+    <mergeCell ref="D55:E55"/>
     <mergeCell ref="C81:E81"/>
     <mergeCell ref="C70:E70"/>
     <mergeCell ref="C71:E71"/>
@@ -2586,6 +2676,26 @@
     <mergeCell ref="D54:E54"/>
     <mergeCell ref="C49:E49"/>
     <mergeCell ref="C50:E50"/>
+    <mergeCell ref="E103:E106"/>
+    <mergeCell ref="F103:G103"/>
+    <mergeCell ref="H103:I103"/>
+    <mergeCell ref="C83:E83"/>
+    <mergeCell ref="C84:E84"/>
+    <mergeCell ref="C85:E85"/>
+    <mergeCell ref="C86:E86"/>
+    <mergeCell ref="B99:I99"/>
+    <mergeCell ref="A94:C95"/>
+    <mergeCell ref="G94:G95"/>
+    <mergeCell ref="D95:F95"/>
+    <mergeCell ref="D94:F94"/>
+    <mergeCell ref="D6:I6"/>
+    <mergeCell ref="D7:I7"/>
+    <mergeCell ref="D8:I8"/>
+    <mergeCell ref="D9:I9"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A9:C9"/>
     <mergeCell ref="C51:E51"/>
     <mergeCell ref="D53:E53"/>
     <mergeCell ref="B39:I39"/>
@@ -2594,67 +2704,6 @@
     <mergeCell ref="C41:E41"/>
     <mergeCell ref="C37:E37"/>
     <mergeCell ref="C38:E38"/>
-    <mergeCell ref="A4:I4"/>
-    <mergeCell ref="B88:D88"/>
-    <mergeCell ref="F88:G88"/>
-    <mergeCell ref="B16:I16"/>
-    <mergeCell ref="B28:I28"/>
-    <mergeCell ref="B47:I47"/>
-    <mergeCell ref="B66:I66"/>
-    <mergeCell ref="B72:I72"/>
-    <mergeCell ref="B79:I79"/>
-    <mergeCell ref="B82:I82"/>
-    <mergeCell ref="B87:D87"/>
-    <mergeCell ref="A66:A71"/>
-    <mergeCell ref="A72:A78"/>
-    <mergeCell ref="A79:A81"/>
-    <mergeCell ref="A82:A86"/>
-    <mergeCell ref="B13:I13"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="C31:E31"/>
-    <mergeCell ref="C32:E32"/>
-    <mergeCell ref="C33:E33"/>
-    <mergeCell ref="C35:E35"/>
-    <mergeCell ref="C36:E36"/>
-    <mergeCell ref="B34:I34"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="B21:I21"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="A16:A20"/>
-    <mergeCell ref="A21:A27"/>
-    <mergeCell ref="A110:F110"/>
-    <mergeCell ref="A111:F111"/>
-    <mergeCell ref="A112:F112"/>
-    <mergeCell ref="A113:F113"/>
-    <mergeCell ref="B101:D101"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="C52:E52"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="A39:A43"/>
-    <mergeCell ref="A44:A46"/>
-    <mergeCell ref="B52:B63"/>
-    <mergeCell ref="C42:E42"/>
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="C45:E45"/>
-    <mergeCell ref="C46:E46"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="D56:E56"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="C48:E48"/>
   </mergeCells>
   <pageMargins left="0.59055118110236227" right="0.19685039370078741" top="0.39370078740157483" bottom="0.19685039370078741" header="0" footer="0"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
@@ -2662,6 +2711,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="f8ce19fc-6d1c-4a32-9ccc-c9d52d339ce3">JDHWM6R55FRK-3-1091</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="f8ce19fc-6d1c-4a32-9ccc-c9d52d339ce3">
+      <Url>http://intra-ecorr.pertamina.com:1043/sites/DIR/_layouts/DocIdRedir.aspx?ID=JDHWM6R55FRK-3-1091</Url>
+      <Description>JDHWM6R55FRK-3-1091</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D3398B66F6FF2D41BB4BC1F9AFA58185" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3a6c582f2b0bd71f194a9173d25feba3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f8ce19fc-6d1c-4a32-9ccc-c9d52d339ce3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bbc7d0c2066ec31eb77a1a91b3421a26" ns2:_="">
     <xsd:import namespace="f8ce19fc-6d1c-4a32-9ccc-c9d52d339ce3"/>
@@ -2806,28 +2867,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocId xmlns="f8ce19fc-6d1c-4a32-9ccc-c9d52d339ce3">JDHWM6R55FRK-3-1091</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="f8ce19fc-6d1c-4a32-9ccc-c9d52d339ce3">
-      <Url>http://intra-ecorr.pertamina.com:1043/sites/DIR/_layouts/DocIdRedir.aspx?ID=JDHWM6R55FRK-3-1091</Url>
-      <Description>JDHWM6R55FRK-3-1091</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -2873,7 +2913,26 @@
 </spe:Receivers>
 </file>
 
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F0FE8FF-1470-4D65-B8CB-44279A87CD25}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="f8ce19fc-6d1c-4a32-9ccc-c9d52d339ce3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50EAB68D-D504-41D1-82F9-E4C3C5838B05}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2891,28 +2950,18 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F0FE8FF-1470-4D65-B8CB-44279A87CD25}">
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{25744CA3-91BF-4923-A10C-D92CF0741E21}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="f8ce19fc-6d1c-4a32-9ccc-c9d52d339ce3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{63767986-64D3-45A1-BF8E-61CD1787B5FF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{25744CA3-91BF-4923-A10C-D92CF0741E21}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>